<commit_message>
Added Test automation info in SRS
</commit_message>
<xml_diff>
--- a/Documents/TestScenarioTemplate.xlsx
+++ b/Documents/TestScenarioTemplate.xlsx
@@ -182,6 +182,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -194,16 +198,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -519,27 +547,27 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -547,33 +575,33 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>